<commit_message>
ajout affichage par liste
</commit_message>
<xml_diff>
--- a/TableauDeBord.xlsx
+++ b/TableauDeBord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Desktop\GitHub\S3D_MyWishList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DA2619-B512-46E4-9710-0DD5AD75E5EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22187677-875A-4AA5-94D9-EF953F163F3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
   <si>
     <t>BOUSSETTA Nael</t>
   </si>
@@ -107,7 +107,7 @@
     <t>Creation de liste</t>
   </si>
   <si>
-    <t xml:space="preserve"> x</t>
+    <t>Affichage par liste</t>
   </si>
 </sst>
 </file>
@@ -639,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="62.5703125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -785,7 +785,7 @@
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="4" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="F7" s="17"/>
       <c r="G7" s="4" t="s">
@@ -798,9 +798,21 @@
       <c r="J7" s="17"/>
     </row>
     <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="B8" s="17"/>
+      <c r="C8" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="D8" s="17"/>
+      <c r="E8" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="F8" s="17"/>
+      <c r="G8" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="H8" s="17"/>
       <c r="J8" s="17"/>
     </row>

</xml_diff>

<commit_message>
mise en place de v4
</commit_message>
<xml_diff>
--- a/TableauDeBord.xlsx
+++ b/TableauDeBord.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PHP\S3D_MyWishList\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Desktop\GitHub\S3D_MyWishList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F18263-BABF-4920-B42A-D6A739BC1D72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18201187-4CBF-486D-A56B-2F93D3424AB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TableauBord" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
   <si>
     <t>BOUSSETTA Nael</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>Partage d'une liste</t>
+  </si>
+  <si>
+    <t>Separation des controleurs</t>
+  </si>
+  <si>
+    <t>V4</t>
   </si>
 </sst>
 </file>
@@ -642,26 +648,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="62.5546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="62.5703125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="62.5546875" style="4"/>
-    <col min="2" max="2" width="1.6640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="62.5546875" style="4"/>
-    <col min="4" max="4" width="1.6640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="62.5546875" style="4"/>
-    <col min="6" max="6" width="1.6640625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="62.5546875" style="4"/>
-    <col min="8" max="8" width="1.6640625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" style="6" customWidth="1"/>
-    <col min="10" max="10" width="1.6640625" style="4" customWidth="1"/>
-    <col min="11" max="16384" width="62.5546875" style="4"/>
+    <col min="1" max="1" width="62.5703125" style="4"/>
+    <col min="2" max="2" width="1.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="62.5703125" style="4"/>
+    <col min="4" max="4" width="1.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="62.5703125" style="4"/>
+    <col min="6" max="6" width="1.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="62.5703125" style="4"/>
+    <col min="8" max="8" width="1.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="1.7109375" style="4" customWidth="1"/>
+    <col min="11" max="16384" width="62.5703125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
@@ -674,7 +680,7 @@
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
     </row>
-    <row r="2" spans="1:10" s="8" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" s="8" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -696,7 +702,7 @@
       </c>
       <c r="J2" s="17"/>
     </row>
-    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -715,7 +721,7 @@
       <c r="H3" s="17"/>
       <c r="J3" s="17"/>
     </row>
-    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -734,7 +740,7 @@
       <c r="H4" s="17"/>
       <c r="J4" s="17"/>
     </row>
-    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -756,7 +762,7 @@
       </c>
       <c r="J5" s="17"/>
     </row>
-    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -778,7 +784,7 @@
       </c>
       <c r="J6" s="17"/>
     </row>
-    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -800,7 +806,7 @@
       </c>
       <c r="J7" s="17"/>
     </row>
-    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -819,167 +825,191 @@
       <c r="H8" s="17"/>
       <c r="J8" s="17"/>
     </row>
-    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="B9" s="17"/>
+      <c r="C9" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="D9" s="17"/>
       <c r="E9" s="4" t="s">
         <v>27</v>
       </c>
       <c r="F9" s="17"/>
+      <c r="G9" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="H9" s="17"/>
       <c r="I9" s="7">
         <v>44203</v>
       </c>
       <c r="J9" s="17"/>
     </row>
-    <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="B10" s="17"/>
+      <c r="C10" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="D10" s="17"/>
+      <c r="E10" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="F10" s="17"/>
+      <c r="G10" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="H10" s="17"/>
+      <c r="I10" s="7">
+        <v>44203</v>
+      </c>
       <c r="J10" s="17"/>
     </row>
-    <row r="11" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="17"/>
       <c r="D11" s="17"/>
       <c r="F11" s="17"/>
       <c r="H11" s="17"/>
       <c r="J11" s="17"/>
     </row>
-    <row r="12" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="17"/>
       <c r="D12" s="17"/>
       <c r="F12" s="17"/>
       <c r="H12" s="17"/>
       <c r="J12" s="17"/>
     </row>
-    <row r="13" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="17"/>
       <c r="D13" s="17"/>
       <c r="F13" s="17"/>
       <c r="H13" s="17"/>
       <c r="J13" s="17"/>
     </row>
-    <row r="14" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="17"/>
       <c r="D14" s="17"/>
       <c r="F14" s="17"/>
       <c r="H14" s="17"/>
       <c r="J14" s="17"/>
     </row>
-    <row r="15" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="17"/>
       <c r="D15" s="17"/>
       <c r="F15" s="17"/>
       <c r="H15" s="17"/>
       <c r="J15" s="17"/>
     </row>
-    <row r="16" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="17"/>
       <c r="D16" s="17"/>
       <c r="F16" s="17"/>
       <c r="H16" s="17"/>
       <c r="J16" s="17"/>
     </row>
-    <row r="17" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="17"/>
       <c r="D17" s="17"/>
       <c r="F17" s="17"/>
       <c r="H17" s="17"/>
       <c r="J17" s="17"/>
     </row>
-    <row r="18" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="17"/>
       <c r="D18" s="17"/>
       <c r="F18" s="17"/>
       <c r="H18" s="17"/>
       <c r="J18" s="17"/>
     </row>
-    <row r="19" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="17"/>
       <c r="D19" s="17"/>
       <c r="F19" s="17"/>
       <c r="H19" s="17"/>
       <c r="J19" s="17"/>
     </row>
-    <row r="20" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="17"/>
       <c r="D20" s="17"/>
       <c r="F20" s="17"/>
       <c r="H20" s="17"/>
       <c r="J20" s="17"/>
     </row>
-    <row r="21" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="17"/>
       <c r="D21" s="17"/>
       <c r="F21" s="17"/>
       <c r="H21" s="17"/>
       <c r="J21" s="17"/>
     </row>
-    <row r="22" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="17"/>
       <c r="D22" s="17"/>
       <c r="F22" s="17"/>
       <c r="H22" s="17"/>
       <c r="J22" s="17"/>
     </row>
-    <row r="23" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="17"/>
       <c r="D23" s="17"/>
       <c r="F23" s="17"/>
       <c r="H23" s="17"/>
       <c r="J23" s="17"/>
     </row>
-    <row r="24" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="17"/>
       <c r="D24" s="17"/>
       <c r="F24" s="17"/>
       <c r="H24" s="17"/>
       <c r="J24" s="17"/>
     </row>
-    <row r="25" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="17"/>
       <c r="D25" s="17"/>
       <c r="F25" s="17"/>
       <c r="H25" s="17"/>
       <c r="J25" s="17"/>
     </row>
-    <row r="26" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="17"/>
       <c r="D26" s="17"/>
       <c r="F26" s="17"/>
       <c r="H26" s="17"/>
       <c r="J26" s="17"/>
     </row>
-    <row r="27" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="17"/>
       <c r="D27" s="17"/>
       <c r="F27" s="17"/>
       <c r="H27" s="17"/>
       <c r="J27" s="17"/>
     </row>
-    <row r="28" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="17"/>
       <c r="D28" s="17"/>
       <c r="F28" s="17"/>
       <c r="H28" s="17"/>
       <c r="J28" s="17"/>
     </row>
-    <row r="29" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="17"/>
       <c r="D29" s="17"/>
       <c r="F29" s="17"/>
       <c r="H29" s="17"/>
       <c r="J29" s="17"/>
     </row>
-    <row r="30" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="17"/>
       <c r="D30" s="17"/>
       <c r="F30" s="17"/>
       <c r="H30" s="17"/>
       <c r="J30" s="17"/>
     </row>
-    <row r="31" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="17"/>
       <c r="D31" s="17"/>
       <c r="F31" s="17"/>
@@ -1062,12 +1092,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="22.6640625" defaultRowHeight="21" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="22.7109375" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="22.6640625" style="5"/>
+    <col min="1" max="16384" width="22.7109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>14</v>
       </c>
@@ -1078,7 +1108,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="42" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="42" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
@@ -1089,7 +1119,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="63" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
@@ -1100,7 +1130,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="42" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="42" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -1108,7 +1138,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="63" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
@@ -1116,7 +1146,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="42" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="42" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
modif tableau de bord
</commit_message>
<xml_diff>
--- a/TableauDeBord.xlsx
+++ b/TableauDeBord.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Desktop\GitHub\S3D_MyWishList\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5344a3cd4eb43387/Bureau/Git/S3D_MyWishList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18201187-4CBF-486D-A56B-2F93D3424AB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{18201187-4CBF-486D-A56B-2F93D3424AB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{10FB605E-194A-434E-AC76-B6AF8D3C71CF}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TableauBord" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
   <si>
     <t>BOUSSETTA Nael</t>
   </si>
@@ -117,6 +117,12 @@
   </si>
   <si>
     <t>V4</t>
+  </si>
+  <si>
+    <t>Modification et suppression des items</t>
+  </si>
+  <si>
+    <t>Modification des listes</t>
   </si>
 </sst>
 </file>
@@ -649,25 +655,25 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="62.5703125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="62.54296875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="62.5703125" style="4"/>
-    <col min="2" max="2" width="1.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="62.5703125" style="4"/>
-    <col min="4" max="4" width="1.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="62.5703125" style="4"/>
-    <col min="6" max="6" width="1.7109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="62.5703125" style="4"/>
-    <col min="8" max="8" width="1.7109375" style="4" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="1.7109375" style="4" customWidth="1"/>
-    <col min="11" max="16384" width="62.5703125" style="4"/>
+    <col min="1" max="1" width="62.54296875" style="4"/>
+    <col min="2" max="2" width="1.7265625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="62.54296875" style="4"/>
+    <col min="4" max="4" width="1.7265625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="62.54296875" style="4"/>
+    <col min="6" max="6" width="1.7265625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="62.54296875" style="4"/>
+    <col min="8" max="8" width="1.7265625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="10.26953125" style="6" customWidth="1"/>
+    <col min="10" max="10" width="1.7265625" style="4" customWidth="1"/>
+    <col min="11" max="16384" width="62.54296875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
@@ -680,7 +686,7 @@
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
     </row>
-    <row r="2" spans="1:10" s="8" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="8" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -702,7 +708,7 @@
       </c>
       <c r="J2" s="17"/>
     </row>
-    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -721,7 +727,7 @@
       <c r="H3" s="17"/>
       <c r="J3" s="17"/>
     </row>
-    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -740,7 +746,7 @@
       <c r="H4" s="17"/>
       <c r="J4" s="17"/>
     </row>
-    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -762,7 +768,7 @@
       </c>
       <c r="J5" s="17"/>
     </row>
-    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -784,9 +790,9 @@
       </c>
       <c r="J6" s="17"/>
     </row>
-    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="B7" s="17"/>
       <c r="C7" s="4" t="s">
@@ -806,7 +812,7 @@
       </c>
       <c r="J7" s="17"/>
     </row>
-    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -825,9 +831,9 @@
       <c r="H8" s="17"/>
       <c r="J8" s="17"/>
     </row>
-    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="B9" s="17"/>
       <c r="C9" s="4" t="s">
@@ -847,7 +853,7 @@
       </c>
       <c r="J9" s="17"/>
     </row>
-    <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
@@ -869,147 +875,147 @@
       </c>
       <c r="J10" s="17"/>
     </row>
-    <row r="11" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="17"/>
       <c r="D11" s="17"/>
       <c r="F11" s="17"/>
       <c r="H11" s="17"/>
       <c r="J11" s="17"/>
     </row>
-    <row r="12" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="17"/>
       <c r="D12" s="17"/>
       <c r="F12" s="17"/>
       <c r="H12" s="17"/>
       <c r="J12" s="17"/>
     </row>
-    <row r="13" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="17"/>
       <c r="D13" s="17"/>
       <c r="F13" s="17"/>
       <c r="H13" s="17"/>
       <c r="J13" s="17"/>
     </row>
-    <row r="14" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="17"/>
       <c r="D14" s="17"/>
       <c r="F14" s="17"/>
       <c r="H14" s="17"/>
       <c r="J14" s="17"/>
     </row>
-    <row r="15" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="17"/>
       <c r="D15" s="17"/>
       <c r="F15" s="17"/>
       <c r="H15" s="17"/>
       <c r="J15" s="17"/>
     </row>
-    <row r="16" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="17"/>
       <c r="D16" s="17"/>
       <c r="F16" s="17"/>
       <c r="H16" s="17"/>
       <c r="J16" s="17"/>
     </row>
-    <row r="17" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="17"/>
       <c r="D17" s="17"/>
       <c r="F17" s="17"/>
       <c r="H17" s="17"/>
       <c r="J17" s="17"/>
     </row>
-    <row r="18" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="17"/>
       <c r="D18" s="17"/>
       <c r="F18" s="17"/>
       <c r="H18" s="17"/>
       <c r="J18" s="17"/>
     </row>
-    <row r="19" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="17"/>
       <c r="D19" s="17"/>
       <c r="F19" s="17"/>
       <c r="H19" s="17"/>
       <c r="J19" s="17"/>
     </row>
-    <row r="20" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="17"/>
       <c r="D20" s="17"/>
       <c r="F20" s="17"/>
       <c r="H20" s="17"/>
       <c r="J20" s="17"/>
     </row>
-    <row r="21" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="17"/>
       <c r="D21" s="17"/>
       <c r="F21" s="17"/>
       <c r="H21" s="17"/>
       <c r="J21" s="17"/>
     </row>
-    <row r="22" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="17"/>
       <c r="D22" s="17"/>
       <c r="F22" s="17"/>
       <c r="H22" s="17"/>
       <c r="J22" s="17"/>
     </row>
-    <row r="23" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="17"/>
       <c r="D23" s="17"/>
       <c r="F23" s="17"/>
       <c r="H23" s="17"/>
       <c r="J23" s="17"/>
     </row>
-    <row r="24" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="17"/>
       <c r="D24" s="17"/>
       <c r="F24" s="17"/>
       <c r="H24" s="17"/>
       <c r="J24" s="17"/>
     </row>
-    <row r="25" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="17"/>
       <c r="D25" s="17"/>
       <c r="F25" s="17"/>
       <c r="H25" s="17"/>
       <c r="J25" s="17"/>
     </row>
-    <row r="26" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="17"/>
       <c r="D26" s="17"/>
       <c r="F26" s="17"/>
       <c r="H26" s="17"/>
       <c r="J26" s="17"/>
     </row>
-    <row r="27" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="17"/>
       <c r="D27" s="17"/>
       <c r="F27" s="17"/>
       <c r="H27" s="17"/>
       <c r="J27" s="17"/>
     </row>
-    <row r="28" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="17"/>
       <c r="D28" s="17"/>
       <c r="F28" s="17"/>
       <c r="H28" s="17"/>
       <c r="J28" s="17"/>
     </row>
-    <row r="29" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="17"/>
       <c r="D29" s="17"/>
       <c r="F29" s="17"/>
       <c r="H29" s="17"/>
       <c r="J29" s="17"/>
     </row>
-    <row r="30" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" s="17"/>
       <c r="D30" s="17"/>
       <c r="F30" s="17"/>
       <c r="H30" s="17"/>
       <c r="J30" s="17"/>
     </row>
-    <row r="31" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" s="17"/>
       <c r="D31" s="17"/>
       <c r="F31" s="17"/>
@@ -1092,12 +1098,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="22.7109375" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="22.7265625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="22.7109375" style="5"/>
+    <col min="1" max="16384" width="22.7265625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>14</v>
       </c>
@@ -1108,7 +1114,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="42" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
@@ -1119,7 +1125,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="63" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
@@ -1130,7 +1136,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="42" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="42" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -1138,7 +1144,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="63" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
@@ -1146,7 +1152,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="42" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="42" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
correction bug mineur pour les items
</commit_message>
<xml_diff>
--- a/TableauDeBord.xlsx
+++ b/TableauDeBord.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5344a3cd4eb43387/Bureau/Git/S3D_MyWishList/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Desktop\GitHub\S3D_MyWishList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_842BB0AA252B807C6FC98388A41831C28DBF4DA1" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E04E2EAF-9989-4D3C-8758-9749CC5A9D9C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1907108-DCD8-4D67-8611-7613689B8F2B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28020" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TableauBord" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
   <si>
     <t>BOUSSETTA Nael</t>
   </si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t>Réservation item</t>
+  </si>
+  <si>
+    <t>Essaie correction AjoutMessage</t>
+  </si>
+  <si>
+    <t>correction bug mineur pour les items</t>
   </si>
 </sst>
 </file>
@@ -680,26 +686,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="62.54296875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="62.5703125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="62.54296875" style="4"/>
-    <col min="2" max="2" width="1.7265625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="62.54296875" style="4"/>
-    <col min="4" max="4" width="1.7265625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="62.54296875" style="4"/>
-    <col min="6" max="6" width="1.7265625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="62.54296875" style="4"/>
-    <col min="8" max="8" width="1.7265625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="10.26953125" style="6" customWidth="1"/>
-    <col min="10" max="10" width="1.7265625" style="4" customWidth="1"/>
-    <col min="11" max="16384" width="62.54296875" style="4"/>
+    <col min="1" max="1" width="62.5703125" style="4"/>
+    <col min="2" max="2" width="1.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="62.5703125" style="4"/>
+    <col min="4" max="4" width="1.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="62.5703125" style="4"/>
+    <col min="6" max="6" width="1.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="62.5703125" style="4"/>
+    <col min="8" max="8" width="1.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="1.7109375" style="4" customWidth="1"/>
+    <col min="11" max="16384" width="62.5703125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
@@ -712,7 +718,7 @@
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
     </row>
-    <row r="2" spans="1:10" s="8" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" s="8" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -734,7 +740,7 @@
       </c>
       <c r="J2" s="17"/>
     </row>
-    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -753,7 +759,7 @@
       <c r="H3" s="17"/>
       <c r="J3" s="17"/>
     </row>
-    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -772,7 +778,7 @@
       <c r="H4" s="17"/>
       <c r="J4" s="17"/>
     </row>
-    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -794,7 +800,7 @@
       </c>
       <c r="J5" s="17"/>
     </row>
-    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
@@ -816,7 +822,7 @@
       </c>
       <c r="J6" s="17"/>
     </row>
-    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>30</v>
       </c>
@@ -838,7 +844,7 @@
       </c>
       <c r="J7" s="17"/>
     </row>
-    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -857,7 +863,7 @@
       <c r="H8" s="17"/>
       <c r="J8" s="17"/>
     </row>
-    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>31</v>
       </c>
@@ -879,7 +885,7 @@
       </c>
       <c r="J9" s="17"/>
     </row>
-    <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>32</v>
       </c>
@@ -901,7 +907,7 @@
       </c>
       <c r="J10" s="17"/>
     </row>
-    <row r="11" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>6</v>
       </c>
@@ -923,146 +929,155 @@
       </c>
       <c r="J11" s="17"/>
     </row>
-    <row r="12" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B12" s="17"/>
       <c r="D12" s="17"/>
       <c r="F12" s="17"/>
+      <c r="G12" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="H12" s="17"/>
       <c r="I12" s="7">
         <v>44208</v>
       </c>
       <c r="J12" s="17"/>
     </row>
-    <row r="13" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="17"/>
       <c r="D13" s="17"/>
       <c r="F13" s="17"/>
+      <c r="G13" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="H13" s="17"/>
+      <c r="I13" s="7">
+        <v>44208</v>
+      </c>
       <c r="J13" s="17"/>
     </row>
-    <row r="14" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="17"/>
       <c r="D14" s="17"/>
       <c r="F14" s="17"/>
       <c r="H14" s="17"/>
       <c r="J14" s="17"/>
     </row>
-    <row r="15" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="17"/>
       <c r="D15" s="17"/>
       <c r="F15" s="17"/>
       <c r="H15" s="17"/>
       <c r="J15" s="17"/>
     </row>
-    <row r="16" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="17"/>
       <c r="D16" s="17"/>
       <c r="F16" s="17"/>
       <c r="H16" s="17"/>
       <c r="J16" s="17"/>
     </row>
-    <row r="17" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="17"/>
       <c r="D17" s="17"/>
       <c r="F17" s="17"/>
       <c r="H17" s="17"/>
       <c r="J17" s="17"/>
     </row>
-    <row r="18" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="17"/>
       <c r="D18" s="17"/>
       <c r="F18" s="17"/>
       <c r="H18" s="17"/>
       <c r="J18" s="17"/>
     </row>
-    <row r="19" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="17"/>
       <c r="D19" s="17"/>
       <c r="F19" s="17"/>
       <c r="H19" s="17"/>
       <c r="J19" s="17"/>
     </row>
-    <row r="20" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="17"/>
       <c r="D20" s="17"/>
       <c r="F20" s="17"/>
       <c r="H20" s="17"/>
       <c r="J20" s="17"/>
     </row>
-    <row r="21" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="17"/>
       <c r="D21" s="17"/>
       <c r="F21" s="17"/>
       <c r="H21" s="17"/>
       <c r="J21" s="17"/>
     </row>
-    <row r="22" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="17"/>
       <c r="D22" s="17"/>
       <c r="F22" s="17"/>
       <c r="H22" s="17"/>
       <c r="J22" s="17"/>
     </row>
-    <row r="23" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="17"/>
       <c r="D23" s="17"/>
       <c r="F23" s="17"/>
       <c r="H23" s="17"/>
       <c r="J23" s="17"/>
     </row>
-    <row r="24" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="17"/>
       <c r="D24" s="17"/>
       <c r="F24" s="17"/>
       <c r="H24" s="17"/>
       <c r="J24" s="17"/>
     </row>
-    <row r="25" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="17"/>
       <c r="D25" s="17"/>
       <c r="F25" s="17"/>
       <c r="H25" s="17"/>
       <c r="J25" s="17"/>
     </row>
-    <row r="26" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="17"/>
       <c r="D26" s="17"/>
       <c r="F26" s="17"/>
       <c r="H26" s="17"/>
       <c r="J26" s="17"/>
     </row>
-    <row r="27" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="17"/>
       <c r="D27" s="17"/>
       <c r="F27" s="17"/>
       <c r="H27" s="17"/>
       <c r="J27" s="17"/>
     </row>
-    <row r="28" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="17"/>
       <c r="D28" s="17"/>
       <c r="F28" s="17"/>
       <c r="H28" s="17"/>
       <c r="J28" s="17"/>
     </row>
-    <row r="29" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="17"/>
       <c r="D29" s="17"/>
       <c r="F29" s="17"/>
       <c r="H29" s="17"/>
       <c r="J29" s="17"/>
     </row>
-    <row r="30" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="17"/>
       <c r="D30" s="17"/>
       <c r="F30" s="17"/>
       <c r="H30" s="17"/>
       <c r="J30" s="17"/>
     </row>
-    <row r="31" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="17"/>
       <c r="D31" s="17"/>
       <c r="F31" s="17"/>
@@ -1158,12 +1173,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="22.7265625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="22.7109375" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="22.7265625" style="5"/>
+    <col min="1" max="16384" width="22.7109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>14</v>
       </c>
@@ -1174,7 +1189,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="42" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
@@ -1185,7 +1200,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="63" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
@@ -1196,7 +1211,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="42" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="42" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -1204,7 +1219,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="63" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
@@ -1212,7 +1227,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="42" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="42" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
ajout CSS + Deconnexion + Connexion
</commit_message>
<xml_diff>
--- a/TableauDeBord.xlsx
+++ b/TableauDeBord.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Desktop\GitHub\S3D_MyWishList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65EE981D-D34F-4607-9895-C6D7739ECE60}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5393C729-2426-4A19-8E9B-68C47B00BC5F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28020" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26010" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TableauBord" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="40">
   <si>
     <t>BOUSSETTA Nael</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>AjoutMessage</t>
+  </si>
+  <si>
+    <t>Deconnexion</t>
   </si>
 </sst>
 </file>
@@ -689,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="62.5703125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1002,7 +1005,13 @@
       <c r="B15" s="17"/>
       <c r="D15" s="17"/>
       <c r="F15" s="17"/>
+      <c r="G15" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="H15" s="17"/>
+      <c r="I15" s="7">
+        <v>44211</v>
+      </c>
       <c r="J15" s="17"/>
     </row>
     <row r="16" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changement avec la connection et maj du tableau des fonctionnalité
</commit_message>
<xml_diff>
--- a/TableauDeBord.xlsx
+++ b/TableauDeBord.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Desktop\GitHub\S3D_MyWishList\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PHP\S3D_MyWishList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B924EDF6-33EE-4750-86F6-FDE9BAED9D64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4920073-57BC-46B9-9689-00B88B59B0E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4965" yWindow="1305" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TableauBord" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="52">
   <si>
     <t>BOUSSETTA Nael</t>
   </si>
@@ -168,6 +168,21 @@
   </si>
   <si>
     <t>amelioration modification</t>
+  </si>
+  <si>
+    <t>Correction de multiple erreurs pour plusieurs</t>
+  </si>
+  <si>
+    <t>personne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adaptation du site en fonction de la </t>
+  </si>
+  <si>
+    <t>connection</t>
+  </si>
+  <si>
+    <t>mise à jour du css</t>
   </si>
 </sst>
 </file>
@@ -713,26 +728,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="62.5703125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="62.5546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="62.5703125" style="4"/>
-    <col min="2" max="2" width="1.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="62.5703125" style="4"/>
-    <col min="4" max="4" width="1.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="62.5703125" style="4"/>
-    <col min="6" max="6" width="1.7109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="62.5703125" style="4"/>
-    <col min="8" max="8" width="1.7109375" style="4" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="1.7109375" style="4" customWidth="1"/>
-    <col min="11" max="16384" width="62.5703125" style="4"/>
+    <col min="1" max="1" width="62.5546875" style="4"/>
+    <col min="2" max="2" width="1.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="62.5546875" style="4"/>
+    <col min="4" max="4" width="1.6640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="62.5546875" style="4"/>
+    <col min="6" max="6" width="1.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="62.5546875" style="4"/>
+    <col min="8" max="8" width="1.6640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" style="6" customWidth="1"/>
+    <col min="10" max="10" width="1.6640625" style="4" customWidth="1"/>
+    <col min="11" max="16384" width="62.5546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
@@ -745,7 +760,7 @@
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
     </row>
-    <row r="2" spans="1:10" s="8" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="8" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -767,7 +782,7 @@
       </c>
       <c r="J2" s="17"/>
     </row>
-    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -786,7 +801,7 @@
       <c r="H3" s="17"/>
       <c r="J3" s="17"/>
     </row>
-    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -805,7 +820,7 @@
       <c r="H4" s="17"/>
       <c r="J4" s="17"/>
     </row>
-    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -827,7 +842,7 @@
       </c>
       <c r="J5" s="17"/>
     </row>
-    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
@@ -849,7 +864,7 @@
       </c>
       <c r="J6" s="17"/>
     </row>
-    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>30</v>
       </c>
@@ -871,7 +886,7 @@
       </c>
       <c r="J7" s="17"/>
     </row>
-    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -890,7 +905,7 @@
       <c r="H8" s="17"/>
       <c r="J8" s="17"/>
     </row>
-    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>31</v>
       </c>
@@ -912,7 +927,7 @@
       </c>
       <c r="J9" s="17"/>
     </row>
-    <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>32</v>
       </c>
@@ -934,7 +949,7 @@
       </c>
       <c r="J10" s="17"/>
     </row>
-    <row r="11" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>6</v>
       </c>
@@ -956,7 +971,7 @@
       </c>
       <c r="J11" s="17"/>
     </row>
-    <row r="12" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>35</v>
       </c>
@@ -978,7 +993,7 @@
       </c>
       <c r="J12" s="17"/>
     </row>
-    <row r="13" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>6</v>
       </c>
@@ -1000,7 +1015,7 @@
       </c>
       <c r="J13" s="17"/>
     </row>
-    <row r="14" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>42</v>
       </c>
@@ -1022,7 +1037,7 @@
       </c>
       <c r="J14" s="17"/>
     </row>
-    <row r="15" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>6</v>
       </c>
@@ -1044,7 +1059,7 @@
       </c>
       <c r="J15" s="17"/>
     </row>
-    <row r="16" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>6</v>
       </c>
@@ -1066,7 +1081,7 @@
       </c>
       <c r="J16" s="17"/>
     </row>
-    <row r="17" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>43</v>
       </c>
@@ -1076,7 +1091,7 @@
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="4" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="F17" s="17"/>
       <c r="G17" s="4" t="s">
@@ -1088,7 +1103,7 @@
       </c>
       <c r="J17" s="17"/>
     </row>
-    <row r="18" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>44</v>
       </c>
@@ -1098,7 +1113,7 @@
       </c>
       <c r="D18" s="17"/>
       <c r="E18" s="4" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="F18" s="17"/>
       <c r="G18" s="4" t="s">
@@ -1110,7 +1125,7 @@
       </c>
       <c r="J18" s="17"/>
     </row>
-    <row r="19" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>6</v>
       </c>
@@ -1120,7 +1135,7 @@
       </c>
       <c r="D19" s="17"/>
       <c r="E19" s="4" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="F19" s="17"/>
       <c r="G19" s="4" t="s">
@@ -1132,7 +1147,7 @@
       </c>
       <c r="J19" s="17"/>
     </row>
-    <row r="20" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>6</v>
       </c>
@@ -1142,7 +1157,7 @@
       </c>
       <c r="D20" s="17"/>
       <c r="E20" s="4" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="F20" s="17"/>
       <c r="G20" s="4" t="s">
@@ -1154,77 +1169,92 @@
       </c>
       <c r="J20" s="17"/>
     </row>
-    <row r="21" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="B21" s="17"/>
+      <c r="C21" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="D21" s="17"/>
+      <c r="E21" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="F21" s="17"/>
+      <c r="G21" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="H21" s="17"/>
+      <c r="I21" s="7">
+        <v>44214</v>
+      </c>
       <c r="J21" s="17"/>
     </row>
-    <row r="22" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="17"/>
       <c r="D22" s="17"/>
       <c r="F22" s="17"/>
       <c r="H22" s="17"/>
       <c r="J22" s="17"/>
     </row>
-    <row r="23" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="17"/>
       <c r="D23" s="17"/>
       <c r="F23" s="17"/>
       <c r="H23" s="17"/>
       <c r="J23" s="17"/>
     </row>
-    <row r="24" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="17"/>
       <c r="D24" s="17"/>
       <c r="F24" s="17"/>
       <c r="H24" s="17"/>
       <c r="J24" s="17"/>
     </row>
-    <row r="25" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="17"/>
       <c r="D25" s="17"/>
       <c r="F25" s="17"/>
       <c r="H25" s="17"/>
       <c r="J25" s="17"/>
     </row>
-    <row r="26" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="17"/>
       <c r="D26" s="17"/>
       <c r="F26" s="17"/>
       <c r="H26" s="17"/>
       <c r="J26" s="17"/>
     </row>
-    <row r="27" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="17"/>
       <c r="D27" s="17"/>
       <c r="F27" s="17"/>
       <c r="H27" s="17"/>
       <c r="J27" s="17"/>
     </row>
-    <row r="28" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="17"/>
       <c r="D28" s="17"/>
       <c r="F28" s="17"/>
       <c r="H28" s="17"/>
       <c r="J28" s="17"/>
     </row>
-    <row r="29" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="17"/>
       <c r="D29" s="17"/>
       <c r="F29" s="17"/>
       <c r="H29" s="17"/>
       <c r="J29" s="17"/>
     </row>
-    <row r="30" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="17"/>
       <c r="D30" s="17"/>
       <c r="F30" s="17"/>
       <c r="H30" s="17"/>
       <c r="J30" s="17"/>
     </row>
-    <row r="31" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="17"/>
       <c r="D31" s="17"/>
       <c r="F31" s="17"/>
@@ -1320,12 +1350,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="22.7109375" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="22.6640625" defaultRowHeight="21" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="22.7109375" style="5"/>
+    <col min="1" max="16384" width="22.6640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>14</v>
       </c>
@@ -1336,7 +1366,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="42" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="42" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
@@ -1347,7 +1377,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="63" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
@@ -1358,7 +1388,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="42" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="42" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -1366,7 +1396,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="63" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
@@ -1374,7 +1404,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="42" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="42" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>23</v>
       </c>

</xml_diff>